<commit_message>
changes to datasets csv
</commit_message>
<xml_diff>
--- a/MetaGxOvarian/datasetsALL.xlsx
+++ b/MetaGxOvarian/datasetsALL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="28340" yWindow="0" windowWidth="14900" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ovarian" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="317">
   <si>
     <t>Dataset</t>
   </si>
@@ -279,9 +279,6 @@
     <t>EXPO</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Expression project for oncology, large dataset of microarray data published by the International Genomics Consortium</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
     <t>PNC</t>
   </si>
   <si>
-    <t>GSE20711, PMID 21910250</t>
-  </si>
-  <si>
     <t>GSE20711</t>
   </si>
   <si>
@@ -967,13 +961,25 @@
   </si>
   <si>
     <t>list of sample replicates across all expression sets</t>
+  </si>
+  <si>
+    <t>Erin Curley ecurley@intgen.org</t>
+  </si>
+  <si>
+    <t>Jaroslav Petr Novak  jaroslav.novak@gmail.com</t>
+  </si>
+  <si>
+    <t>Pulication_date</t>
+  </si>
+  <si>
+    <t>Publication_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -997,6 +1003,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1015,17 +1038,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1355,15 +1393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="36.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1379,22 +1420,28 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>178</v>
+      <c r="B2" s="2">
+        <v>22348002</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1405,22 +1452,28 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2">
         <v>129</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10572</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>12449</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>178</v>
+      <c r="B3">
+        <v>16996261</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1431,22 +1484,28 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3">
         <v>54</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>9544</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>11276</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>178</v>
+      <c r="B4">
+        <v>19486012</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1457,22 +1516,28 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4">
         <v>53</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>13667</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>15952</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>178</v>
+      <c r="B5">
+        <v>19192944</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1483,22 +1548,28 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5">
         <v>157</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>13846</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>20870</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>178</v>
+      <c r="B6">
+        <v>19294737</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1509,22 +1580,28 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6">
         <v>80</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>12752</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>20967</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>178</v>
+      <c r="B7">
+        <v>20300634</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1535,22 +1612,28 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7">
         <v>110</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>19596</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>30936</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>178</v>
+      <c r="B8">
+        <v>19962670</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -1561,22 +1644,28 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8">
         <v>63</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>20282</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>42447</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>178</v>
+      <c r="B9">
+        <v>20547991</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1587,22 +1676,28 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9">
         <v>70</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>20339</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>54253</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>178</v>
+      <c r="B10">
+        <v>20492709</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1613,22 +1708,28 @@
       <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10">
         <v>140</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>20282</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>42447</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>178</v>
+      <c r="B11" s="3" t="s">
+        <v>313</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1639,22 +1740,25 @@
       <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11">
         <v>204</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>20282</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>42447</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>178</v>
+      <c r="B12">
+        <v>18593951</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -1665,22 +1769,28 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12">
         <v>195</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>12752</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>20967</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="J12">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>178</v>
+      <c r="B13">
+        <v>22492981</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -1691,22 +1801,28 @@
       <c r="E13" t="s">
         <v>36</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13">
         <v>103</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>359</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>363</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="J13">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>37</v>
       </c>
-      <c r="B14" t="s">
-        <v>178</v>
+      <c r="B14">
+        <v>22348014</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -1717,22 +1833,28 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14">
         <v>58</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>20282</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>42447</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="J14">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
-        <v>178</v>
+      <c r="B15">
+        <v>22241791</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -1743,22 +1865,28 @@
       <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G15">
         <v>260</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>19596</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>30936</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="J15">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>178</v>
+      <c r="B16">
+        <v>22241791</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -1769,22 +1897,28 @@
       <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G16">
         <v>40</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>19596</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>30936</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
-        <v>178</v>
+      <c r="B17">
+        <v>17418409</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -1795,22 +1929,28 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17">
         <v>103</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>12752</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>20967</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="J17">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16">
       <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
-        <v>178</v>
+      <c r="B18" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -1821,22 +1961,25 @@
       <c r="E18" t="s">
         <v>44</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18">
         <v>66</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>5342</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>6407</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>178</v>
+      <c r="B19">
+        <v>18698038</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
@@ -1847,17 +1990,23 @@
       <c r="E19" t="s">
         <v>25</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19">
         <v>285</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>20282</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>42447</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="J19">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1873,17 +2022,20 @@
       <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="F20" t="s">
-        <v>178</v>
+      <c r="F20" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="G20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>176</v>
+      </c>
+      <c r="I20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1899,17 +2051,20 @@
       <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21">
         <v>117</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>12752</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>20967</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1925,23 +2080,23 @@
       <c r="E22" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
-        <v>178</v>
+      <c r="F22" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>176</v>
+      </c>
+      <c r="I22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
-        <v>178</v>
-      </c>
       <c r="C23" t="s">
         <v>49</v>
       </c>
@@ -1951,23 +2106,23 @@
       <c r="E23" t="s">
         <v>51</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23">
         <v>578</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>12833</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>21260</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
-        <v>178</v>
-      </c>
       <c r="C24" t="s">
         <v>52</v>
       </c>
@@ -1977,18 +2132,22 @@
       <c r="E24" t="s">
         <v>53</v>
       </c>
-      <c r="F24" t="s">
-        <v>178</v>
+      <c r="F24" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="G24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="I24" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1999,15 +2158,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2035,8 +2194,11 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -2064,8 +2226,11 @@
       <c r="I2">
         <v>21169</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2093,8 +2258,11 @@
       <c r="I3">
         <v>42447</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -2122,8 +2290,11 @@
       <c r="I4">
         <v>42447</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2151,8 +2322,11 @@
       <c r="I5">
         <v>42447</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2180,8 +2354,11 @@
       <c r="I6">
         <v>12085</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -2209,8 +2386,11 @@
       <c r="I7">
         <v>45490</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -2238,8 +2418,11 @@
       <c r="I8">
         <v>42447</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -2267,13 +2450,16 @@
       <c r="I9">
         <v>20967</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16">
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" t="s">
-        <v>85</v>
+      <c r="B10" s="3" t="s">
+        <v>313</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -2285,7 +2471,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10">
         <v>353</v>
@@ -2297,24 +2483,24 @@
         <v>42447</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <v>17659439</v>
       </c>
       <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
         <v>88</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>89</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>90</v>
-      </c>
-      <c r="F11" t="s">
-        <v>91</v>
       </c>
       <c r="G11">
         <v>150</v>
@@ -2325,25 +2511,28 @@
       <c r="I11">
         <v>6064</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12">
         <v>19688261</v>
       </c>
       <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
         <v>93</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
         <v>94</v>
-      </c>
-      <c r="E12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" t="s">
-        <v>95</v>
       </c>
       <c r="G12">
         <v>53</v>
@@ -2354,22 +2543,25 @@
       <c r="I12">
         <v>26536</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13">
         <v>18498629</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13">
         <v>129</v>
@@ -2380,16 +2572,19 @@
       <c r="I13">
         <v>42447</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14">
         <v>12747878</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
@@ -2398,7 +2593,7 @@
         <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>88</v>
@@ -2409,25 +2604,28 @@
       <c r="I14">
         <v>280</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15">
         <v>18430221</v>
       </c>
       <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
         <v>103</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>104</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>105</v>
-      </c>
-      <c r="F15" t="s">
-        <v>106</v>
       </c>
       <c r="G15">
         <v>143</v>
@@ -2438,25 +2636,28 @@
       <c r="I15">
         <v>11154</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>17452630</v>
       </c>
       <c r="C16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
         <v>108</v>
       </c>
-      <c r="D16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" t="s">
-        <v>109</v>
-      </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16">
         <v>105</v>
@@ -2467,16 +2668,19 @@
       <c r="I16">
         <v>22008</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <v>18593943</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>60</v>
@@ -2485,7 +2689,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17">
         <v>200</v>
@@ -2496,25 +2700,28 @@
       <c r="I17">
         <v>20967</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18">
         <v>20064235</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
         <v>60</v>
       </c>
       <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" t="s">
         <v>115</v>
-      </c>
-      <c r="F18" t="s">
-        <v>116</v>
       </c>
       <c r="G18">
         <v>230</v>
@@ -2525,25 +2732,28 @@
       <c r="I18">
         <v>20967</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19">
         <v>19960244</v>
       </c>
       <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>119</v>
-      </c>
-      <c r="F19" t="s">
-        <v>120</v>
       </c>
       <c r="G19">
         <v>75</v>
@@ -2554,16 +2764,19 @@
       <c r="I19">
         <v>19048</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20">
         <v>16896004</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
@@ -2572,7 +2785,7 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20">
         <v>129</v>
@@ -2583,16 +2796,19 @@
       <c r="I20">
         <v>21169</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>16049480</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
         <v>60</v>
@@ -2601,7 +2817,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G21">
         <v>99</v>
@@ -2612,25 +2828,28 @@
       <c r="I21">
         <v>20967</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>18592372</v>
       </c>
       <c r="C22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" t="s">
         <v>128</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>129</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>130</v>
-      </c>
-      <c r="F22" t="s">
-        <v>131</v>
       </c>
       <c r="G22">
         <v>152</v>
@@ -2641,16 +2860,19 @@
       <c r="I22">
         <v>14288</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23">
         <v>18636107</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
         <v>60</v>
@@ -2659,7 +2881,7 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G23">
         <v>183</v>
@@ -2670,25 +2892,28 @@
       <c r="I23">
         <v>20967</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24">
         <v>12917485</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G24">
         <v>99</v>
@@ -2699,25 +2924,28 @@
       <c r="I24">
         <v>5154</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" t="s">
         <v>137</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>138</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>139</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" t="s">
         <v>140</v>
-      </c>
-      <c r="E25" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" t="s">
-        <v>141</v>
       </c>
       <c r="G25">
         <v>337</v>
@@ -2728,16 +2956,19 @@
       <c r="I25">
         <v>14960</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26">
+        <v>21910250</v>
+      </c>
+      <c r="C26" t="s">
         <v>142</v>
-      </c>
-      <c r="B26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" t="s">
-        <v>144</v>
       </c>
       <c r="D26" t="s">
         <v>60</v>
@@ -2754,25 +2985,28 @@
       <c r="I26">
         <v>42447</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B27">
         <v>16280042</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D27" t="s">
         <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G27">
         <v>159</v>
@@ -2783,25 +3017,28 @@
       <c r="I27">
         <v>36178</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B28">
         <v>12829800</v>
       </c>
       <c r="C28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" t="s">
         <v>150</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" t="s">
-        <v>151</v>
-      </c>
-      <c r="F28" t="s">
-        <v>152</v>
       </c>
       <c r="G28">
         <v>118</v>
@@ -2812,13 +3049,16 @@
       <c r="I28">
         <v>3663</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
         <v>60</v>
@@ -2835,10 +3075,13 @@
       <c r="I29">
         <v>21169</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B30">
         <v>18498629</v>
@@ -2858,16 +3101,19 @@
       <c r="I30">
         <v>42369</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B31">
         <v>17545524</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D31" t="s">
         <v>60</v>
@@ -2876,7 +3122,7 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G31">
         <v>198</v>
@@ -2887,25 +3133,28 @@
       <c r="I31">
         <v>20967</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" t="s">
         <v>159</v>
-      </c>
-      <c r="B32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" t="s">
-        <v>161</v>
       </c>
       <c r="G32">
         <v>162</v>
@@ -2916,25 +3165,28 @@
       <c r="I32">
         <v>8015</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33">
         <v>20813035</v>
       </c>
       <c r="C33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" t="s">
         <v>163</v>
-      </c>
-      <c r="D33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" t="s">
-        <v>164</v>
-      </c>
-      <c r="F33" t="s">
-        <v>165</v>
       </c>
       <c r="G33">
         <v>305</v>
@@ -2945,16 +3197,19 @@
       <c r="I33">
         <v>5420</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" t="s">
         <v>166</v>
-      </c>
-      <c r="B34" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" t="s">
-        <v>168</v>
       </c>
       <c r="D34" t="s">
         <v>60</v>
@@ -2963,7 +3218,7 @@
         <v>60</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G34">
         <v>133</v>
@@ -2974,16 +3229,19 @@
       <c r="I34">
         <v>36084</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B35">
         <v>16141321</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D35" t="s">
         <v>60</v>
@@ -2992,7 +3250,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G35">
         <v>251</v>
@@ -3003,16 +3261,19 @@
       <c r="I35">
         <v>36178</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" t="s">
         <v>173</v>
-      </c>
-      <c r="B36" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" t="s">
-        <v>175</v>
       </c>
       <c r="D36" t="s">
         <v>60</v>
@@ -3021,7 +3282,7 @@
         <v>60</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G36">
         <v>344</v>
@@ -3032,16 +3293,22 @@
       <c r="I36">
         <v>21169</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>175</v>
+      </c>
+      <c r="B37">
+        <v>22522925</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G37">
         <v>2136</v>
@@ -3052,11 +3319,17 @@
       <c r="I37">
         <v>36155</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>49</v>
       </c>
+      <c r="B38">
+        <v>25267403</v>
+      </c>
       <c r="D38" t="s">
         <v>49</v>
       </c>
@@ -3072,9 +3345,13 @@
       <c r="I38">
         <v>19504</v>
       </c>
+      <c r="J38">
+        <v>2014</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3095,682 +3372,682 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
         <v>185</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>186</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>187</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>188</v>
-      </c>
-      <c r="E2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" t="s">
         <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
         <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" t="s">
         <v>197</v>
-      </c>
-      <c r="B5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" t="s">
         <v>200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" t="s">
         <v>203</v>
-      </c>
-      <c r="B7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" t="s">
         <v>208</v>
-      </c>
-      <c r="B9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" t="s">
-        <v>209</v>
-      </c>
-      <c r="F9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F10" t="s">
         <v>211</v>
-      </c>
-      <c r="B10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" t="s">
-        <v>195</v>
-      </c>
-      <c r="D10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" t="s">
-        <v>212</v>
-      </c>
-      <c r="F10" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F11" t="s">
         <v>214</v>
-      </c>
-      <c r="B11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" t="s">
         <v>217</v>
-      </c>
-      <c r="B12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" t="s">
         <v>220</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F13" t="s">
         <v>221</v>
-      </c>
-      <c r="C13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" t="s">
-        <v>222</v>
-      </c>
-      <c r="F13" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" t="s">
         <v>224</v>
-      </c>
-      <c r="B14" t="s">
-        <v>221</v>
-      </c>
-      <c r="C14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" t="s">
-        <v>225</v>
-      </c>
-      <c r="F14" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>226</v>
+      </c>
+      <c r="F15" t="s">
         <v>227</v>
-      </c>
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" t="s">
-        <v>192</v>
-      </c>
-      <c r="E15" t="s">
-        <v>228</v>
-      </c>
-      <c r="F15" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" t="s">
         <v>234</v>
       </c>
-      <c r="B18" t="s">
+      <c r="F18" t="s">
         <v>235</v>
-      </c>
-      <c r="C18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" t="s">
-        <v>236</v>
-      </c>
-      <c r="F18" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" t="s">
+        <v>237</v>
+      </c>
+      <c r="F19" t="s">
         <v>238</v>
-      </c>
-      <c r="B19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" t="s">
-        <v>192</v>
-      </c>
-      <c r="E19" t="s">
-        <v>239</v>
-      </c>
-      <c r="F19" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F21" t="s">
         <v>243</v>
-      </c>
-      <c r="B21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C21" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" t="s">
-        <v>192</v>
-      </c>
-      <c r="E21" t="s">
-        <v>244</v>
-      </c>
-      <c r="F21" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F22" t="s">
         <v>246</v>
-      </c>
-      <c r="B22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" t="s">
-        <v>247</v>
-      </c>
-      <c r="F22" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>250</v>
+      </c>
+      <c r="F24" t="s">
         <v>251</v>
-      </c>
-      <c r="B24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C24" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E24" t="s">
-        <v>252</v>
-      </c>
-      <c r="F24" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" t="s">
+        <v>253</v>
+      </c>
+      <c r="F25" t="s">
         <v>254</v>
-      </c>
-      <c r="B25" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" t="s">
-        <v>195</v>
-      </c>
-      <c r="D25" t="s">
-        <v>192</v>
-      </c>
-      <c r="E25" t="s">
-        <v>255</v>
-      </c>
-      <c r="F25" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" t="s">
+        <v>256</v>
+      </c>
+      <c r="F26" t="s">
         <v>257</v>
-      </c>
-      <c r="B26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" t="s">
-        <v>195</v>
-      </c>
-      <c r="D26" t="s">
-        <v>192</v>
-      </c>
-      <c r="E26" t="s">
-        <v>258</v>
-      </c>
-      <c r="F26" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" t="s">
+        <v>259</v>
+      </c>
+      <c r="F27" t="s">
         <v>260</v>
-      </c>
-      <c r="B27" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" t="s">
-        <v>195</v>
-      </c>
-      <c r="D27" t="s">
-        <v>192</v>
-      </c>
-      <c r="E27" t="s">
-        <v>261</v>
-      </c>
-      <c r="F27" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F28" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F31" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F33" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3788,7 +4065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -3796,542 +4073,542 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
         <v>185</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>186</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>187</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>188</v>
-      </c>
-      <c r="E2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" t="s">
         <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
         <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" t="s">
         <v>277</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>278</v>
-      </c>
-      <c r="C6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E6" t="s">
-        <v>279</v>
-      </c>
-      <c r="F6" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" t="s">
         <v>285</v>
-      </c>
-      <c r="B9" t="s">
-        <v>286</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" t="s">
-        <v>236</v>
-      </c>
-      <c r="F9" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" t="s">
         <v>290</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>291</v>
-      </c>
-      <c r="C11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" t="s">
-        <v>292</v>
-      </c>
-      <c r="F11" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" t="s">
         <v>297</v>
-      </c>
-      <c r="B14" t="s">
-        <v>298</v>
-      </c>
-      <c r="C14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" t="s">
-        <v>236</v>
-      </c>
-      <c r="F14" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>299</v>
+      </c>
+      <c r="F15" t="s">
         <v>300</v>
-      </c>
-      <c r="B15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" t="s">
-        <v>192</v>
-      </c>
-      <c r="E15" t="s">
-        <v>301</v>
-      </c>
-      <c r="F15" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
         <v>234</v>
       </c>
-      <c r="B16" t="s">
-        <v>291</v>
-      </c>
-      <c r="C16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" t="s">
-        <v>236</v>
-      </c>
       <c r="F16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" t="s">
+        <v>306</v>
+      </c>
+      <c r="F20" t="s">
         <v>307</v>
-      </c>
-      <c r="B20" t="s">
-        <v>298</v>
-      </c>
-      <c r="C20" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" t="s">
-        <v>308</v>
-      </c>
-      <c r="F20" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B21" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" t="s">
+        <v>259</v>
+      </c>
+      <c r="F22" t="s">
         <v>260</v>
-      </c>
-      <c r="B22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" t="s">
-        <v>261</v>
-      </c>
-      <c r="F22" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F26" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>